<commit_message>
push sua dia danh
</commit_message>
<xml_diff>
--- a/API/wwwroot/DLL/CQT_DiaDanh.xlsx
+++ b/API/wwwroot/DLL/CQT_DiaDanh.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Mã cơ quan thuế</t>
   </si>
@@ -43,12 +43,21 @@
   <si>
     <t>08</t>
   </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,6 +80,12 @@
       <family val="1"/>
       <charset val="163"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -86,7 +101,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -109,6 +124,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -124,11 +154,11 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -412,8 +442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B65" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -422,7 +452,7 @@
     <col min="2" max="2" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -440,112 +470,112 @@
       <c r="A3" s="3">
         <v>10300</v>
       </c>
-      <c r="B3" s="2">
-        <v>31</v>
+      <c r="B3" s="4" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>10700</v>
       </c>
-      <c r="B4" s="2">
-        <v>30</v>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>10900</v>
       </c>
-      <c r="B5" s="2">
-        <v>33</v>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>11100</v>
       </c>
-      <c r="B6" s="2">
-        <v>35</v>
+      <c r="B6" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>11300</v>
       </c>
-      <c r="B7" s="2">
-        <v>36</v>
+      <c r="B7" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>11500</v>
       </c>
-      <c r="B8" s="2">
-        <v>34</v>
+      <c r="B8" s="4">
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>11700</v>
       </c>
-      <c r="B9" s="2">
-        <v>37</v>
+      <c r="B9" s="4">
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>20100</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>2</v>
+      <c r="B10" s="5">
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>20300</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>3</v>
+      <c r="B11" s="5">
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>20500</v>
       </c>
-      <c r="B12" s="2">
-        <v>10</v>
+      <c r="B12" s="5">
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>20700</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>4</v>
+      <c r="B13" s="5">
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>20900</v>
       </c>
-      <c r="B14" s="2">
-        <v>20</v>
+      <c r="B14" s="5">
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>21100</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>5</v>
+      <c r="B15" s="5">
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>21300</v>
       </c>
-      <c r="B16" s="2">
-        <v>15</v>
+      <c r="B16" s="5">
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.3">
@@ -553,30 +583,30 @@
         <v>21500</v>
       </c>
       <c r="B17" s="5">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>21700</v>
       </c>
-      <c r="B18" s="2">
-        <v>25</v>
+      <c r="B18" s="5">
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>21900</v>
       </c>
-      <c r="B19" s="2">
-        <v>26</v>
+      <c r="B19" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>22100</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="5">
         <v>24</v>
       </c>
     </row>
@@ -584,352 +614,352 @@
       <c r="A21" s="3">
         <v>22300</v>
       </c>
-      <c r="B21" s="2">
-        <v>27</v>
+      <c r="B21" s="5">
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>22500</v>
       </c>
-      <c r="B22" s="2">
-        <v>22</v>
+      <c r="B22" s="5">
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>30100</v>
       </c>
-      <c r="B23" s="2">
-        <v>11</v>
+      <c r="B23" s="5">
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>30200</v>
       </c>
-      <c r="B24" s="2">
-        <v>12</v>
+      <c r="B24" s="5">
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>30300</v>
       </c>
-      <c r="B25" s="2">
-        <v>14</v>
+      <c r="B25" s="5">
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>30500</v>
       </c>
-      <c r="B26" s="2">
-        <v>17</v>
+      <c r="B26" s="5">
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>40100</v>
       </c>
-      <c r="B27" s="2">
-        <v>38</v>
+      <c r="B27" s="5">
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>40300</v>
       </c>
-      <c r="B28" s="2">
-        <v>40</v>
+      <c r="B28" s="5">
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>40500</v>
       </c>
-      <c r="B29" s="2">
-        <v>42</v>
+      <c r="B29" s="5">
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>40700</v>
       </c>
-      <c r="B30" s="2">
-        <v>44</v>
+      <c r="B30" s="5">
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>40900</v>
       </c>
-      <c r="B31" s="2">
-        <v>45</v>
+      <c r="B31" s="5">
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>41100</v>
       </c>
-      <c r="B32" s="2">
-        <v>46</v>
+      <c r="B32" s="5">
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>50100</v>
       </c>
-      <c r="B33" s="2">
-        <v>48</v>
+      <c r="B33" s="4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>50300</v>
       </c>
-      <c r="B34" s="2">
-        <v>49</v>
+      <c r="B34" s="5">
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>50500</v>
       </c>
-      <c r="B35" s="2">
-        <v>51</v>
+      <c r="B35" s="5">
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>50700</v>
       </c>
-      <c r="B36" s="2">
-        <v>52</v>
+      <c r="B36" s="5">
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>50900</v>
       </c>
-      <c r="B37" s="2">
-        <v>54</v>
+      <c r="B37" s="5">
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>51100</v>
       </c>
-      <c r="B38" s="2">
-        <v>56</v>
+      <c r="B38" s="5">
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>60100</v>
       </c>
-      <c r="B39" s="2">
-        <v>62</v>
+      <c r="B39" s="5">
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>60300</v>
       </c>
-      <c r="B40" s="2">
-        <v>64</v>
+      <c r="B40" s="5">
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>60500</v>
       </c>
-      <c r="B41" s="2">
-        <v>66</v>
+      <c r="B41" s="5">
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>60600</v>
       </c>
-      <c r="B42" s="2">
-        <v>67</v>
+      <c r="B42" s="4">
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>70100</v>
       </c>
-      <c r="B43" s="2">
-        <v>79</v>
+      <c r="B43" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>70300</v>
       </c>
-      <c r="B44" s="2">
-        <v>68</v>
+      <c r="B44" s="5">
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>70500</v>
       </c>
-      <c r="B45" s="2">
-        <v>58</v>
+      <c r="B45" s="5">
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>70700</v>
       </c>
-      <c r="B46" s="2">
-        <v>70</v>
+      <c r="B46" s="5">
+        <v>38</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>70900</v>
       </c>
-      <c r="B47" s="2">
-        <v>72</v>
+      <c r="B47" s="5">
+        <v>39</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>71100</v>
       </c>
-      <c r="B48" s="2">
-        <v>74</v>
+      <c r="B48" s="5">
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>71300</v>
       </c>
-      <c r="B49" s="2">
-        <v>75</v>
+      <c r="B49" s="5">
+        <v>36</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>71500</v>
       </c>
-      <c r="B50" s="2">
-        <v>60</v>
+      <c r="B50" s="5">
+        <v>34</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>71700</v>
       </c>
-      <c r="B51" s="2">
-        <v>77</v>
+      <c r="B51" s="5">
+        <v>35</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>80100</v>
       </c>
-      <c r="B52" s="2">
-        <v>80</v>
+      <c r="B52" s="5">
+        <v>11</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>80300</v>
       </c>
-      <c r="B53" s="2">
-        <v>87</v>
+      <c r="B53" s="5">
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>80500</v>
       </c>
-      <c r="B54" s="2">
-        <v>89</v>
+      <c r="B54" s="5">
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>80700</v>
       </c>
-      <c r="B55" s="2">
-        <v>82</v>
+      <c r="B55" s="5">
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>80900</v>
       </c>
-      <c r="B56" s="2">
-        <v>86</v>
+      <c r="B56" s="5">
+        <v>15</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>81100</v>
       </c>
-      <c r="B57" s="2">
-        <v>83</v>
+      <c r="B57" s="5">
+        <v>13</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>81300</v>
       </c>
-      <c r="B58" s="2">
-        <v>91</v>
+      <c r="B58" s="5">
+        <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>81500</v>
       </c>
-      <c r="B59" s="2">
-        <v>92</v>
+      <c r="B59" s="5">
+        <v>18</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>81600</v>
       </c>
-      <c r="B60" s="2">
-        <v>93</v>
+      <c r="B60" s="5">
+        <v>63</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>81700</v>
       </c>
-      <c r="B61" s="2">
-        <v>84</v>
+      <c r="B61" s="5">
+        <v>21</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>81900</v>
       </c>
-      <c r="B62" s="2">
-        <v>94</v>
+      <c r="B62" s="5">
+        <v>22</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>82100</v>
       </c>
-      <c r="B63" s="2">
-        <v>95</v>
+      <c r="B63" s="5">
+        <v>19</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>82300</v>
       </c>
-      <c r="B64" s="2">
-        <v>96</v>
+      <c r="B64" s="5">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>